<commit_message>
Final version of AN200 documents
</commit_message>
<xml_diff>
--- a/src/Pickles/MIL_pickles/Output/AN200/AN200_TestScript_All.xlsx
+++ b/src/Pickles/MIL_pickles/Output/AN200/AN200_TestScript_All.xlsx
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="1756">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1755">
   <x:si>
     <x:t>AddROI</x:t>
   </x:si>
@@ -1349,7 +1349,7 @@
     <x:t>the grades menu is displayed</x:t>
   </x:si>
   <x:si>
-    <x:t>the grade can be set to D3 or D4</x:t>
+    <x:t>the grade can be set to D</x:t>
   </x:si>
   <x:si>
     <x:t>DenyAssignmentOfDentineGrades</x:t>
@@ -1367,7 +1367,7 @@
     <x:t>I left-click on a caries roi</x:t>
   </x:si>
   <x:si>
-    <x:t>the grade cannot be set to D3 or D4</x:t>
+    <x:t>the grade cannot be set to D</x:t>
   </x:si>
   <x:si>
     <x:t>FeatureTour</x:t>
@@ -4497,7 +4497,7 @@
     <x:t>both enamel and dentine caries are displayed</x:t>
   </x:si>
   <x:si>
-    <x:t>I can change the grade of a caries roi to D3 or D4</x:t>
+    <x:t>I can change the grade of a caries roi to D</x:t>
   </x:si>
   <x:si>
     <x:t>DisableDentine</x:t>
@@ -4512,7 +4512,7 @@
     <x:t>only enamel caries are displayed</x:t>
   </x:si>
   <x:si>
-    <x:t>I am unable to change the grade to D3 or D4</x:t>
+    <x:t>I am unable to change the grade to D</x:t>
   </x:si>
   <x:si>
     <x:t>EnterFeedback</x:t>
@@ -4772,13 +4772,10 @@
     <x:t>the information includes the UDI Device Identifier</x:t>
   </x:si>
   <x:si>
-    <x:t>the information includes the CE mark</x:t>
+    <x:t>the information includes the UKCA mark</x:t>
   </x:si>
   <x:si>
     <x:t>the information includes the manufacturer details</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the information includes the CE representative details</x:t>
   </x:si>
   <x:si>
     <x:t>the information includes the date of manufacture</x:t>
@@ -5908,7 +5905,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
-        <x:v>1753</x:v>
+        <x:v>1752</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -6108,7 +6105,7 @@
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="1" t="s">
-        <x:v>1754</x:v>
+        <x:v>1753</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
@@ -6138,7 +6135,7 @@
     </x:row>
     <x:row r="47" spans="1:2">
       <x:c r="A47" s="1" t="s">
-        <x:v>1755</x:v>
+        <x:v>1754</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
@@ -6258,12 +6255,12 @@
     </x:row>
     <x:row r="71" spans="1:2">
       <x:c r="B71" s="6" t="s">
-        <x:v>1557</x:v>
+        <x:v>1556</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:2">
       <x:c r="B72" s="6" t="s">
-        <x:v>1571</x:v>
+        <x:v>1570</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:2">
@@ -6278,12 +6275,12 @@
     </x:row>
     <x:row r="75" spans="1:2">
       <x:c r="B75" s="6" t="s">
-        <x:v>1614</x:v>
+        <x:v>1613</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:2">
       <x:c r="B76" s="6" t="s">
-        <x:v>1626</x:v>
+        <x:v>1625</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:2">
@@ -6298,37 +6295,37 @@
     </x:row>
     <x:row r="79" spans="1:2">
       <x:c r="B79" s="6" t="s">
-        <x:v>1660</x:v>
+        <x:v>1659</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:2">
       <x:c r="B80" s="6" t="s">
-        <x:v>1666</x:v>
+        <x:v>1665</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:2">
       <x:c r="B81" s="6" t="s">
-        <x:v>1688</x:v>
+        <x:v>1687</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:2">
       <x:c r="B82" s="6" t="s">
-        <x:v>1698</x:v>
+        <x:v>1697</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:2">
       <x:c r="B83" s="6" t="s">
-        <x:v>1719</x:v>
+        <x:v>1718</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:2">
       <x:c r="B84" s="6" t="s">
-        <x:v>1732</x:v>
+        <x:v>1731</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:2">
       <x:c r="B85" s="6" t="s">
-        <x:v>1744</x:v>
+        <x:v>1743</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -22485,7 +22482,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D27"/>
+  <x:dimension ref="A1:D26"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -22603,31 +22600,31 @@
         <x:v>1548</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
+    <x:row r="19" spans="1:4">
+      <x:c r="B19" s="1" t="s">
         <x:v>1549</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
-      <x:c r="B20" s="1" t="s">
+      <x:c r="B20" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
         <x:v>1550</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="B21" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C21" s="2" t="s">
+    <x:row r="21" spans="1:4"/>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
         <x:v>1551</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:4"/>
     <x:row r="23" spans="1:4">
       <x:c r="C23" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>1552</x:v>
@@ -22635,7 +22632,7 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="C24" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
         <x:v>1553</x:v>
@@ -22655,14 +22652,6 @@
       </x:c>
       <x:c r="D26" s="0" t="s">
         <x:v>1555</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="C27" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>1556</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -22687,7 +22676,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1557</x:v>
+        <x:v>1556</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -22695,17 +22684,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1558</x:v>
+        <x:v>1557</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1559</x:v>
+        <x:v>1558</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1560</x:v>
+        <x:v>1559</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -22713,7 +22702,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1561</x:v>
+        <x:v>1560</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -22730,7 +22719,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1562</x:v>
+        <x:v>1561</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -22738,7 +22727,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1563</x:v>
+        <x:v>1562</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -22746,7 +22735,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1564</x:v>
+        <x:v>1563</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -22754,7 +22743,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>1565</x:v>
+        <x:v>1564</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -22762,12 +22751,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>1566</x:v>
+        <x:v>1565</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
       <x:c r="B15" s="1" t="s">
-        <x:v>1567</x:v>
+        <x:v>1566</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -22775,7 +22764,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C16" s="2" t="s">
-        <x:v>1568</x:v>
+        <x:v>1567</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4"/>
@@ -22792,7 +22781,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1569</x:v>
+        <x:v>1568</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -22800,7 +22789,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1563</x:v>
+        <x:v>1562</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -22808,7 +22797,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1564</x:v>
+        <x:v>1563</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -22816,7 +22805,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>1565</x:v>
+        <x:v>1564</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -22824,7 +22813,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>1570</x:v>
+        <x:v>1569</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -22849,7 +22838,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1571</x:v>
+        <x:v>1570</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -22857,17 +22846,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1572</x:v>
+        <x:v>1571</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1573</x:v>
+        <x:v>1572</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1574</x:v>
+        <x:v>1573</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -22875,7 +22864,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1575</x:v>
+        <x:v>1574</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -22900,7 +22889,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1576</x:v>
+        <x:v>1575</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -22908,12 +22897,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1577</x:v>
+        <x:v>1576</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="B13" s="1" t="s">
-        <x:v>1578</x:v>
+        <x:v>1577</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -22921,7 +22910,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>1579</x:v>
+        <x:v>1578</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -22938,7 +22927,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1580</x:v>
+        <x:v>1579</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -22946,7 +22935,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1581</x:v>
+        <x:v>1580</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -22954,7 +22943,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1582</x:v>
+        <x:v>1581</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -22962,7 +22951,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1583</x:v>
+        <x:v>1582</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -22970,7 +22959,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1582</x:v>
+        <x:v>1581</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23003,17 +22992,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1584</x:v>
+        <x:v>1583</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1585</x:v>
+        <x:v>1584</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1586</x:v>
+        <x:v>1585</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23021,7 +23010,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1587</x:v>
+        <x:v>1586</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23038,7 +23027,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1588</x:v>
+        <x:v>1587</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -23046,12 +23035,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1589</x:v>
+        <x:v>1588</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>1590</x:v>
+        <x:v>1589</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -23059,7 +23048,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>1591</x:v>
+        <x:v>1590</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -23076,7 +23065,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>1592</x:v>
+        <x:v>1591</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -23084,7 +23073,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1593</x:v>
+        <x:v>1592</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -23092,7 +23081,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1594</x:v>
+        <x:v>1593</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -23100,12 +23089,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1595</x:v>
+        <x:v>1594</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="B21" s="1" t="s">
-        <x:v>1596</x:v>
+        <x:v>1595</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -23113,7 +23102,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C22" s="2" t="s">
-        <x:v>1597</x:v>
+        <x:v>1596</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4"/>
@@ -23130,7 +23119,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>1598</x:v>
+        <x:v>1597</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -23138,7 +23127,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>1599</x:v>
+        <x:v>1598</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4">
@@ -23146,7 +23135,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>1600</x:v>
+        <x:v>1599</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23179,17 +23168,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1601</x:v>
+        <x:v>1600</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1602</x:v>
+        <x:v>1601</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1603</x:v>
+        <x:v>1602</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23197,7 +23186,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1604</x:v>
+        <x:v>1603</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23206,7 +23195,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>1605</x:v>
+        <x:v>1604</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -23214,7 +23203,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1606</x:v>
+        <x:v>1605</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -23222,12 +23211,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1607</x:v>
+        <x:v>1606</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>1608</x:v>
+        <x:v>1607</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -23235,7 +23224,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>1609</x:v>
+        <x:v>1608</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -23244,7 +23233,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>1605</x:v>
+        <x:v>1604</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -23252,7 +23241,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>1610</x:v>
+        <x:v>1609</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -23260,7 +23249,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1607</x:v>
+        <x:v>1606</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -23273,7 +23262,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C20" s="2" t="s">
-        <x:v>1611</x:v>
+        <x:v>1610</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4"/>
@@ -23298,7 +23287,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>1612</x:v>
+        <x:v>1611</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
@@ -23306,7 +23295,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>1613</x:v>
+        <x:v>1612</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23331,7 +23320,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1614</x:v>
+        <x:v>1613</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -23339,17 +23328,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1615</x:v>
+        <x:v>1614</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1616</x:v>
+        <x:v>1615</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1617</x:v>
+        <x:v>1616</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23357,7 +23346,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1618</x:v>
+        <x:v>1617</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23366,7 +23355,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>1619</x:v>
+        <x:v>1618</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -23374,12 +23363,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1620</x:v>
+        <x:v>1619</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="B11" s="1" t="s">
-        <x:v>1621</x:v>
+        <x:v>1620</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -23387,7 +23376,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C12" s="2" t="s">
-        <x:v>1622</x:v>
+        <x:v>1621</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4"/>
@@ -23396,7 +23385,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>1623</x:v>
+        <x:v>1622</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -23404,7 +23393,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>1624</x:v>
+        <x:v>1623</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -23412,7 +23401,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>1625</x:v>
+        <x:v>1624</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23437,7 +23426,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1626</x:v>
+        <x:v>1625</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -23445,17 +23434,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1627</x:v>
+        <x:v>1626</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1628</x:v>
+        <x:v>1627</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1629</x:v>
+        <x:v>1628</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23463,7 +23452,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1630</x:v>
+        <x:v>1629</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23480,7 +23469,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1631</x:v>
+        <x:v>1630</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -23488,7 +23477,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1632</x:v>
+        <x:v>1631</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -23496,7 +23485,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1633</x:v>
+        <x:v>1632</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -23504,12 +23493,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>1634</x:v>
+        <x:v>1633</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="B14" s="1" t="s">
-        <x:v>1635</x:v>
+        <x:v>1634</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -23517,7 +23506,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C15" s="2" t="s">
-        <x:v>1636</x:v>
+        <x:v>1635</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4"/>
@@ -23550,7 +23539,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1637</x:v>
+        <x:v>1636</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -23558,7 +23547,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1638</x:v>
+        <x:v>1637</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -23566,7 +23555,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>1639</x:v>
+        <x:v>1638</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23599,17 +23588,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1640</x:v>
+        <x:v>1639</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1641</x:v>
+        <x:v>1640</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1642</x:v>
+        <x:v>1641</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23617,7 +23606,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1643</x:v>
+        <x:v>1642</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23642,12 +23631,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1644</x:v>
+        <x:v>1643</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>1645</x:v>
+        <x:v>1644</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -23655,7 +23644,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>1646</x:v>
+        <x:v>1645</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -23680,7 +23669,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1644</x:v>
+        <x:v>1643</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -23688,7 +23677,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1647</x:v>
+        <x:v>1646</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -23704,7 +23693,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1648</x:v>
+        <x:v>1647</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -23712,12 +23701,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1649</x:v>
+        <x:v>1648</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="B23" s="1" t="s">
-        <x:v>1650</x:v>
+        <x:v>1649</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
@@ -23725,7 +23714,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C24" s="2" t="s">
-        <x:v>1651</x:v>
+        <x:v>1650</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4"/>
@@ -23742,7 +23731,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>1652</x:v>
+        <x:v>1651</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
@@ -23750,7 +23739,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>1653</x:v>
+        <x:v>1652</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23783,12 +23772,12 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1654</x:v>
+        <x:v>1653</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1655</x:v>
+        <x:v>1654</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -23801,7 +23790,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1656</x:v>
+        <x:v>1655</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23831,7 +23820,7 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>1657</x:v>
+        <x:v>1656</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -23839,7 +23828,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>1658</x:v>
+        <x:v>1657</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -23856,7 +23845,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>1659</x:v>
+        <x:v>1658</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -23889,7 +23878,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1660</x:v>
+        <x:v>1659</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -23897,12 +23886,12 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1661</x:v>
+        <x:v>1660</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1662</x:v>
+        <x:v>1661</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -23915,7 +23904,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1663</x:v>
+        <x:v>1662</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23924,7 +23913,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>1664</x:v>
+        <x:v>1663</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -23932,7 +23921,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1665</x:v>
+        <x:v>1664</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -23957,7 +23946,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1666</x:v>
+        <x:v>1665</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -23965,17 +23954,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1667</x:v>
+        <x:v>1666</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1668</x:v>
+        <x:v>1667</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1669</x:v>
+        <x:v>1668</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -23983,7 +23972,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1670</x:v>
+        <x:v>1669</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -23992,7 +23981,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>1671</x:v>
+        <x:v>1670</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -24000,7 +23989,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1672</x:v>
+        <x:v>1671</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -24008,7 +23997,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1673</x:v>
+        <x:v>1672</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -24016,7 +24005,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1674</x:v>
+        <x:v>1673</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -24032,12 +24021,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>1675</x:v>
+        <x:v>1674</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
       <x:c r="B15" s="1" t="s">
-        <x:v>1676</x:v>
+        <x:v>1675</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -24045,7 +24034,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C16" s="2" t="s">
-        <x:v>1677</x:v>
+        <x:v>1676</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4"/>
@@ -24054,7 +24043,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1671</x:v>
+        <x:v>1670</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -24062,7 +24051,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1672</x:v>
+        <x:v>1671</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -24070,7 +24059,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1678</x:v>
+        <x:v>1677</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -24078,7 +24067,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1679</x:v>
+        <x:v>1678</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -24086,7 +24075,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>1680</x:v>
+        <x:v>1679</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -24094,12 +24083,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>1681</x:v>
+        <x:v>1680</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="B25" s="1" t="s">
-        <x:v>1682</x:v>
+        <x:v>1681</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -24107,7 +24096,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C26" s="2" t="s">
-        <x:v>1683</x:v>
+        <x:v>1682</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4"/>
@@ -24116,7 +24105,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>1671</x:v>
+        <x:v>1670</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -24124,7 +24113,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>1672</x:v>
+        <x:v>1671</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
@@ -24132,7 +24121,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>1684</x:v>
+        <x:v>1683</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:4">
@@ -24140,7 +24129,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>1674</x:v>
+        <x:v>1673</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
@@ -24156,12 +24145,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>1675</x:v>
+        <x:v>1674</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4">
       <x:c r="B35" s="1" t="s">
-        <x:v>1685</x:v>
+        <x:v>1684</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4">
@@ -24169,7 +24158,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C36" s="2" t="s">
-        <x:v>1686</x:v>
+        <x:v>1685</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:4"/>
@@ -24178,7 +24167,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>1671</x:v>
+        <x:v>1670</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:4">
@@ -24186,7 +24175,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D39" s="0" t="s">
-        <x:v>1672</x:v>
+        <x:v>1671</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4">
@@ -24194,7 +24183,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
-        <x:v>1687</x:v>
+        <x:v>1686</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4">
@@ -24202,7 +24191,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D41" s="0" t="s">
-        <x:v>1674</x:v>
+        <x:v>1673</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:4">
@@ -24218,7 +24207,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>1675</x:v>
+        <x:v>1674</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -24243,7 +24232,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1688</x:v>
+        <x:v>1687</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -24251,12 +24240,12 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1689</x:v>
+        <x:v>1688</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1690</x:v>
+        <x:v>1689</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -24269,7 +24258,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1691</x:v>
+        <x:v>1690</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -24294,7 +24283,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1692</x:v>
+        <x:v>1691</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -24302,7 +24291,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1693</x:v>
+        <x:v>1692</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -24315,7 +24304,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>1694</x:v>
+        <x:v>1693</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -24340,7 +24329,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1695</x:v>
+        <x:v>1694</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -24348,7 +24337,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1696</x:v>
+        <x:v>1695</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -24356,7 +24345,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1697</x:v>
+        <x:v>1696</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -25089,7 +25078,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1698</x:v>
+        <x:v>1697</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -25097,17 +25086,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1699</x:v>
+        <x:v>1698</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1700</x:v>
+        <x:v>1699</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1701</x:v>
+        <x:v>1700</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -25124,7 +25113,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>1702</x:v>
+        <x:v>1701</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -25145,7 +25134,7 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>1703</x:v>
+        <x:v>1702</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -25153,7 +25142,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>1704</x:v>
+        <x:v>1703</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -25162,7 +25151,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>1705</x:v>
+        <x:v>1704</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -25178,12 +25167,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1706</x:v>
+        <x:v>1705</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="B19" s="1" t="s">
-        <x:v>1707</x:v>
+        <x:v>1706</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -25191,7 +25180,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C20" s="2" t="s">
-        <x:v>1708</x:v>
+        <x:v>1707</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4"/>
@@ -25200,7 +25189,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>1705</x:v>
+        <x:v>1704</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -25216,7 +25205,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>1706</x:v>
+        <x:v>1705</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
@@ -25224,7 +25213,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>1709</x:v>
+        <x:v>1708</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -25232,12 +25221,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>1710</x:v>
+        <x:v>1709</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
       <x:c r="B28" s="1" t="s">
-        <x:v>1711</x:v>
+        <x:v>1710</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -25245,7 +25234,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C29" s="2" t="s">
-        <x:v>1712</x:v>
+        <x:v>1711</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4"/>
@@ -25254,7 +25243,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>1705</x:v>
+        <x:v>1704</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
@@ -25270,7 +25259,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>1706</x:v>
+        <x:v>1705</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:4">
@@ -25278,12 +25267,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>1713</x:v>
+        <x:v>1712</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4">
       <x:c r="B36" s="1" t="s">
-        <x:v>1714</x:v>
+        <x:v>1713</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:4">
@@ -25291,7 +25280,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C37" s="2" t="s">
-        <x:v>1715</x:v>
+        <x:v>1714</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:4"/>
@@ -25300,7 +25289,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D39" s="0" t="s">
-        <x:v>1705</x:v>
+        <x:v>1704</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4">
@@ -25308,7 +25297,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
-        <x:v>1716</x:v>
+        <x:v>1715</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4">
@@ -25329,7 +25318,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C44" s="2" t="s">
-        <x:v>1717</x:v>
+        <x:v>1716</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:4"/>
@@ -25338,7 +25327,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D46" s="0" t="s">
-        <x:v>1705</x:v>
+        <x:v>1704</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:4">
@@ -25346,7 +25335,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D47" s="0" t="s">
-        <x:v>1718</x:v>
+        <x:v>1717</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:4">
@@ -25354,7 +25343,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>1706</x:v>
+        <x:v>1705</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -25379,7 +25368,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1719</x:v>
+        <x:v>1718</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -25387,17 +25376,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1720</x:v>
+        <x:v>1719</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1721</x:v>
+        <x:v>1720</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1722</x:v>
+        <x:v>1721</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -25405,7 +25394,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1723</x:v>
+        <x:v>1722</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -25422,7 +25411,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1724</x:v>
+        <x:v>1723</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -25430,7 +25419,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1725</x:v>
+        <x:v>1724</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -25438,7 +25427,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1726</x:v>
+        <x:v>1725</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -25446,12 +25435,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>1727</x:v>
+        <x:v>1726</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="B14" s="1" t="s">
-        <x:v>1728</x:v>
+        <x:v>1727</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -25459,7 +25448,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C15" s="2" t="s">
-        <x:v>1729</x:v>
+        <x:v>1728</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4"/>
@@ -25476,7 +25465,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1730</x:v>
+        <x:v>1729</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -25484,7 +25473,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1725</x:v>
+        <x:v>1724</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -25492,7 +25481,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1726</x:v>
+        <x:v>1725</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -25500,7 +25489,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>1731</x:v>
+        <x:v>1730</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -25525,7 +25514,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1732</x:v>
+        <x:v>1731</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -25533,17 +25522,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1733</x:v>
+        <x:v>1732</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1734</x:v>
+        <x:v>1733</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1735</x:v>
+        <x:v>1734</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -25551,7 +25540,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1736</x:v>
+        <x:v>1735</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -25576,7 +25565,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1737</x:v>
+        <x:v>1736</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -25584,12 +25573,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1738</x:v>
+        <x:v>1737</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="B13" s="1" t="s">
-        <x:v>1739</x:v>
+        <x:v>1738</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -25597,7 +25586,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>1740</x:v>
+        <x:v>1739</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -25622,7 +25611,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1741</x:v>
+        <x:v>1740</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -25630,7 +25619,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1742</x:v>
+        <x:v>1741</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -25638,7 +25627,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>1743</x:v>
+        <x:v>1742</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -25663,7 +25652,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>1744</x:v>
+        <x:v>1743</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -25671,17 +25660,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1745</x:v>
+        <x:v>1744</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>1746</x:v>
+        <x:v>1745</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>1747</x:v>
+        <x:v>1746</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -25689,7 +25678,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>1748</x:v>
+        <x:v>1747</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -25706,7 +25695,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>1562</x:v>
+        <x:v>1561</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -25714,7 +25703,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>1749</x:v>
+        <x:v>1748</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -25722,12 +25711,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>1750</x:v>
+        <x:v>1749</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="B13" s="1" t="s">
-        <x:v>1751</x:v>
+        <x:v>1750</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -25735,7 +25724,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>1752</x:v>
+        <x:v>1751</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -25752,7 +25741,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>1569</x:v>
+        <x:v>1568</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -25760,7 +25749,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>1749</x:v>
+        <x:v>1748</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -25768,7 +25757,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>1750</x:v>
+        <x:v>1749</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>